<commit_message>
Fixed bug in add_letter_dirs and add_author_dirs
</commit_message>
<xml_diff>
--- a/data/painters.xlsx
+++ b/data/painters.xlsx
@@ -38465,7 +38465,7 @@
       </c>
       <c r="B2057" t="inlineStr">
         <is>
-          <t>Master Of 1540s</t>
+          <t>Master Of 1540S</t>
         </is>
       </c>
     </row>
@@ -39235,7 +39235,7 @@
       </c>
       <c r="B2134" t="inlineStr">
         <is>
-          <t xml:space="preserve">Master Of The Pietà</t>
+          <t>Master Of The Pietà</t>
         </is>
       </c>
     </row>

</xml_diff>